<commit_message>
sql számításos hibák javítása
</commit_message>
<xml_diff>
--- a/sql/Match3.xlsx
+++ b/sql/Match3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\zarovizsga_2021\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DC37A3-1F9D-4511-92EC-20D0E180D1C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1802CC-EB52-40DD-BEB4-1164BC756E5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feladat adatai" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Csontos Krisztián</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>tipus</t>
+  </si>
+  <si>
+    <t>jatekos1_ranglistapont</t>
+  </si>
+  <si>
+    <t>jatekos2_ranglistapont</t>
   </si>
 </sst>
 </file>
@@ -194,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -220,6 +226,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -772,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,7 +813,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">RANDBETWEEN(0,7)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -828,7 +837,7 @@
       </c>
       <c r="C4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -840,7 +849,7 @@
       </c>
       <c r="C5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -852,7 +861,7 @@
       </c>
       <c r="C6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -864,7 +873,7 @@
       </c>
       <c r="C7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -876,7 +885,7 @@
       </c>
       <c r="C8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -888,7 +897,7 @@
       </c>
       <c r="C9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -900,7 +909,7 @@
       </c>
       <c r="C10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -912,7 +921,7 @@
       </c>
       <c r="C11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -924,7 +933,7 @@
       </c>
       <c r="C12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -936,7 +945,7 @@
       </c>
       <c r="C13" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -948,7 +957,7 @@
       </c>
       <c r="C14" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -960,7 +969,7 @@
       </c>
       <c r="C15" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -972,7 +981,7 @@
       </c>
       <c r="C16" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -984,7 +993,7 @@
       </c>
       <c r="C17" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -996,7 +1005,7 @@
       </c>
       <c r="C18" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1008,7 +1017,7 @@
       </c>
       <c r="C19" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1020,7 +1029,7 @@
       </c>
       <c r="C20" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1032,7 +1041,7 @@
       </c>
       <c r="C21" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1044,7 +1053,7 @@
       </c>
       <c r="C22" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1056,7 +1065,7 @@
       </c>
       <c r="C23" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1068,7 +1077,7 @@
       </c>
       <c r="C24" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1080,7 +1089,7 @@
       </c>
       <c r="C25" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1092,7 +1101,7 @@
       </c>
       <c r="C26" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1104,7 +1113,7 @@
       </c>
       <c r="C27" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1116,7 +1125,7 @@
       </c>
       <c r="C28" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1128,7 +1137,7 @@
       </c>
       <c r="C29" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1140,7 +1149,7 @@
       </c>
       <c r="C30" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1152,7 +1161,7 @@
       </c>
       <c r="C31" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1164,7 +1173,7 @@
       </c>
       <c r="C32" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1188,7 +1197,7 @@
       </c>
       <c r="C34" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1200,7 +1209,7 @@
       </c>
       <c r="C35" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1212,7 +1221,7 @@
       </c>
       <c r="C36" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1224,7 +1233,7 @@
       </c>
       <c r="C37" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1236,7 +1245,7 @@
       </c>
       <c r="C38" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1272,7 +1281,7 @@
       </c>
       <c r="C41" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1284,7 +1293,7 @@
       </c>
       <c r="C42" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1296,7 +1305,7 @@
       </c>
       <c r="C43" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1308,7 +1317,7 @@
       </c>
       <c r="C44" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1320,7 +1329,7 @@
       </c>
       <c r="C45" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1332,7 +1341,7 @@
       </c>
       <c r="C46" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1344,7 +1353,7 @@
       </c>
       <c r="C47" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1368,7 +1377,7 @@
       </c>
       <c r="C49" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1380,7 +1389,7 @@
       </c>
       <c r="C50" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1392,7 +1401,7 @@
       </c>
       <c r="C51" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1404,7 +1413,7 @@
       </c>
       <c r="C52" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1416,7 +1425,7 @@
       </c>
       <c r="C53" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1428,7 +1437,7 @@
       </c>
       <c r="C54" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1464,7 +1473,7 @@
       </c>
       <c r="C57" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1476,7 +1485,7 @@
       </c>
       <c r="C58" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1488,7 +1497,7 @@
       </c>
       <c r="C59" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1500,7 +1509,7 @@
       </c>
       <c r="C60" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1512,7 +1521,7 @@
       </c>
       <c r="C61" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1524,7 +1533,7 @@
       </c>
       <c r="C62" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1536,7 +1545,7 @@
       </c>
       <c r="C63" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1548,7 +1557,7 @@
       </c>
       <c r="C64" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1575,10 +1584,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B77560E-6709-4717-9C95-7FAA7073CA20}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1588,9 +1597,11 @@
     <col min="4" max="4" width="13.5546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="14.21875" style="4" customWidth="1"/>
     <col min="6" max="9" width="8.88671875" style="4"/>
+    <col min="11" max="11" width="20.44140625" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
@@ -1618,8 +1629,14 @@
       <c r="I1" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1647,8 +1664,17 @@
       <c r="I2" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K2" s="12" t="str">
+        <f>IMSUB(D2,E2)</f>
+        <v>300</v>
+      </c>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12" t="str">
+        <f>IMSUB(E2,D2)</f>
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1676,8 +1702,17 @@
       <c r="I3" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K3" s="12" t="str">
+        <f t="shared" ref="K3:K21" si="0">IMSUB(D3,E3)</f>
+        <v>200</v>
+      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12" t="str">
+        <f t="shared" ref="M3:M21" si="1">IMSUB(E3,D3)</f>
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1705,8 +1740,17 @@
       <c r="I4" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K4" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1734,8 +1778,17 @@
       <c r="I5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K5" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1763,8 +1816,17 @@
       <c r="I6" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K6" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1792,8 +1854,17 @@
       <c r="I7" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K7" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1821,8 +1892,17 @@
       <c r="I8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K8" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-500</v>
+      </c>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1850,8 +1930,17 @@
       <c r="I9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K9" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1879,8 +1968,17 @@
       <c r="I10" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K10" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1908,8 +2006,17 @@
       <c r="I11" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K11" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-300</v>
+      </c>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1937,8 +2044,17 @@
       <c r="I12" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K12" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1966,8 +2082,17 @@
       <c r="I13" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K13" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1995,8 +2120,17 @@
       <c r="I14" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K14" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-700</v>
+      </c>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2024,8 +2158,17 @@
       <c r="I15" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K15" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>-400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2053,8 +2196,17 @@
       <c r="I16" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K16" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-700</v>
+      </c>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2082,8 +2234,17 @@
       <c r="I17" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K17" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2111,8 +2272,17 @@
       <c r="I18" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K18" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2140,8 +2310,17 @@
       <c r="I19" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K19" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-400</v>
+      </c>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2169,8 +2348,17 @@
       <c r="I20" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K20" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-200</v>
+      </c>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2197,6 +2385,31 @@
       </c>
       <c r="I21" s="4">
         <v>1</v>
+      </c>
+      <c r="K21" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-900</v>
+      </c>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K23" s="12">
+        <f>SUM(K2:K22)</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12">
+        <f>SUM(K23:L23)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2305,15 +2518,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentum" ma:contentTypeID="0x010100D5CD1BAABE4B864D99EEDEB0815AF0BD" ma:contentTypeVersion="9" ma:contentTypeDescription="Új dokumentum létrehozása." ma:contentTypeScope="" ma:versionID="40cfcc79a81fe85593353a5e3e8f4000">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a076746e-6b52-4ee0-bd34-9f0723d04451" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a1acbe04eb5be477cef83f3a6104cc73" ns2:_="">
     <xsd:import namespace="a076746e-6b52-4ee0-bd34-9f0723d04451"/>
@@ -2491,6 +2695,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{303689F6-2334-4750-8807-CA54D5A92A7F}">
   <ds:schemaRefs>
@@ -2501,14 +2714,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8FA63BD-FF56-41E8-A8F1-B982A33E165C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BFD4E4D-4659-4D12-82C6-9C04FFB9DB53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2524,4 +2729,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8FA63BD-FF56-41E8-A8F1-B982A33E165C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>